<commit_message>
everything working as intended for sure now
</commit_message>
<xml_diff>
--- a/car_info.xlsx
+++ b/car_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="132">
   <si>
     <t>URL</t>
   </si>
@@ -313,13 +313,19 @@
     <t>Black paint with orange interior highlights</t>
   </si>
   <si>
+    <t>Price not found</t>
+  </si>
+  <si>
+    <t>SOLD</t>
+  </si>
+  <si>
     <t>£143,995</t>
   </si>
   <si>
     <t>£177,000</t>
   </si>
   <si>
-    <t>£240,000</t>
+    <t>£235,000</t>
   </si>
   <si>
     <t>£97,995</t>
@@ -343,27 +349,21 @@
     <t>£269,999</t>
   </si>
   <si>
-    <t>Price not found</t>
-  </si>
-  <si>
-    <t>£208,000</t>
+    <t>£132,995</t>
+  </si>
+  <si>
+    <t>£199,000</t>
   </si>
   <si>
     <t>£229,995</t>
   </si>
   <si>
-    <t>£137,604</t>
-  </si>
-  <si>
     <t>£89,900</t>
   </si>
   <si>
     <t>£83,500</t>
   </si>
   <si>
-    <t>£65,995</t>
-  </si>
-  <si>
     <t>£69,950</t>
   </si>
   <si>
@@ -376,9 +376,6 @@
     <t>£136,990</t>
   </si>
   <si>
-    <t>£147,999</t>
-  </si>
-  <si>
     <t>£124,850</t>
   </si>
   <si>
@@ -388,34 +385,16 @@
     <t>£144,890</t>
   </si>
   <si>
-    <t>£235,000</t>
-  </si>
-  <si>
-    <t>SOLD</t>
-  </si>
-  <si>
-    <t>£79,660</t>
-  </si>
-  <si>
     <t>£214,995</t>
   </si>
   <si>
-    <t>£199,000</t>
-  </si>
-  <si>
-    <t>£79,460</t>
+    <t>£79,360</t>
   </si>
   <si>
     <t>£134,995</t>
   </si>
   <si>
     <t>£134,948</t>
-  </si>
-  <si>
-    <t>£79,360</t>
-  </si>
-  <si>
-    <t>£132,995</t>
   </si>
   <si>
     <t>£87,990</t>
@@ -885,44 +864,44 @@
       <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="F2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" t="s">
-        <v>99</v>
-      </c>
-      <c r="N2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>99</v>
+      <c r="F2">
+        <v>143995</v>
+      </c>
+      <c r="G2">
+        <v>143995</v>
+      </c>
+      <c r="H2">
+        <v>143995</v>
+      </c>
+      <c r="I2">
+        <v>143995</v>
+      </c>
+      <c r="J2">
+        <v>143995</v>
+      </c>
+      <c r="K2">
+        <v>143995</v>
+      </c>
+      <c r="L2">
+        <v>143995</v>
+      </c>
+      <c r="M2">
+        <v>143995</v>
+      </c>
+      <c r="N2">
+        <v>143995</v>
+      </c>
+      <c r="O2">
+        <v>143995</v>
+      </c>
+      <c r="P2">
+        <v>143995</v>
+      </c>
+      <c r="Q2">
+        <v>143995</v>
       </c>
       <c r="R2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -941,44 +920,44 @@
       <c r="E3" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L3" t="s">
-        <v>100</v>
-      </c>
-      <c r="M3" t="s">
-        <v>100</v>
-      </c>
-      <c r="N3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P3" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>100</v>
+      <c r="F3">
+        <v>177000</v>
+      </c>
+      <c r="G3">
+        <v>177000</v>
+      </c>
+      <c r="H3">
+        <v>177000</v>
+      </c>
+      <c r="I3">
+        <v>177000</v>
+      </c>
+      <c r="J3">
+        <v>177000</v>
+      </c>
+      <c r="K3">
+        <v>177000</v>
+      </c>
+      <c r="L3">
+        <v>177000</v>
+      </c>
+      <c r="M3">
+        <v>177000</v>
+      </c>
+      <c r="N3">
+        <v>177000</v>
+      </c>
+      <c r="O3">
+        <v>177000</v>
+      </c>
+      <c r="P3">
+        <v>177000</v>
+      </c>
+      <c r="Q3">
+        <v>177000</v>
       </c>
       <c r="R3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -997,44 +976,44 @@
       <c r="E4" t="s">
         <v>91</v>
       </c>
-      <c r="F4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H4" t="s">
-        <v>124</v>
-      </c>
-      <c r="I4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J4" t="s">
-        <v>124</v>
-      </c>
-      <c r="K4" t="s">
-        <v>124</v>
-      </c>
-      <c r="L4" t="s">
-        <v>124</v>
-      </c>
-      <c r="M4" t="s">
-        <v>124</v>
-      </c>
-      <c r="N4" t="s">
-        <v>124</v>
-      </c>
-      <c r="O4" t="s">
-        <v>124</v>
-      </c>
-      <c r="P4" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>124</v>
+      <c r="F4">
+        <v>240000</v>
+      </c>
+      <c r="G4">
+        <v>235000</v>
+      </c>
+      <c r="H4">
+        <v>235000</v>
+      </c>
+      <c r="I4">
+        <v>235000</v>
+      </c>
+      <c r="J4">
+        <v>235000</v>
+      </c>
+      <c r="K4">
+        <v>235000</v>
+      </c>
+      <c r="L4">
+        <v>235000</v>
+      </c>
+      <c r="M4">
+        <v>235000</v>
+      </c>
+      <c r="N4">
+        <v>235000</v>
+      </c>
+      <c r="O4">
+        <v>235000</v>
+      </c>
+      <c r="P4">
+        <v>235000</v>
+      </c>
+      <c r="Q4">
+        <v>235000</v>
       </c>
       <c r="R4" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1053,44 +1032,44 @@
       <c r="E5" t="s">
         <v>92</v>
       </c>
-      <c r="F5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L5" t="s">
-        <v>102</v>
-      </c>
-      <c r="M5" t="s">
-        <v>102</v>
-      </c>
-      <c r="N5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O5" t="s">
-        <v>102</v>
-      </c>
-      <c r="P5" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>102</v>
+      <c r="F5">
+        <v>97995</v>
+      </c>
+      <c r="G5">
+        <v>97995</v>
+      </c>
+      <c r="H5">
+        <v>97995</v>
+      </c>
+      <c r="I5">
+        <v>97995</v>
+      </c>
+      <c r="J5">
+        <v>97995</v>
+      </c>
+      <c r="K5">
+        <v>97995</v>
+      </c>
+      <c r="L5">
+        <v>97995</v>
+      </c>
+      <c r="M5">
+        <v>97995</v>
+      </c>
+      <c r="N5">
+        <v>97995</v>
+      </c>
+      <c r="O5">
+        <v>97995</v>
+      </c>
+      <c r="P5">
+        <v>97995</v>
+      </c>
+      <c r="Q5">
+        <v>97995</v>
       </c>
       <c r="R5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1109,44 +1088,44 @@
       <c r="E6" t="s">
         <v>90</v>
       </c>
-      <c r="F6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J6" t="s">
-        <v>103</v>
-      </c>
-      <c r="K6" t="s">
-        <v>103</v>
-      </c>
-      <c r="L6" t="s">
-        <v>103</v>
-      </c>
-      <c r="M6" t="s">
-        <v>103</v>
-      </c>
-      <c r="N6" t="s">
-        <v>103</v>
-      </c>
-      <c r="O6" t="s">
-        <v>103</v>
-      </c>
-      <c r="P6" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>103</v>
+      <c r="F6">
+        <v>179995</v>
+      </c>
+      <c r="G6">
+        <v>179995</v>
+      </c>
+      <c r="H6">
+        <v>179995</v>
+      </c>
+      <c r="I6">
+        <v>179995</v>
+      </c>
+      <c r="J6">
+        <v>179995</v>
+      </c>
+      <c r="K6">
+        <v>179995</v>
+      </c>
+      <c r="L6">
+        <v>179995</v>
+      </c>
+      <c r="M6">
+        <v>179995</v>
+      </c>
+      <c r="N6">
+        <v>179995</v>
+      </c>
+      <c r="O6">
+        <v>179995</v>
+      </c>
+      <c r="P6">
+        <v>179995</v>
+      </c>
+      <c r="Q6">
+        <v>179995</v>
       </c>
       <c r="R6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1165,44 +1144,44 @@
       <c r="E7" t="s">
         <v>93</v>
       </c>
-      <c r="F7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L7" t="s">
-        <v>104</v>
-      </c>
-      <c r="M7" t="s">
-        <v>104</v>
-      </c>
-      <c r="N7" t="s">
-        <v>104</v>
-      </c>
-      <c r="O7" t="s">
-        <v>104</v>
-      </c>
-      <c r="P7" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>104</v>
+      <c r="F7">
+        <v>287970</v>
+      </c>
+      <c r="G7">
+        <v>287970</v>
+      </c>
+      <c r="H7">
+        <v>287970</v>
+      </c>
+      <c r="I7">
+        <v>287970</v>
+      </c>
+      <c r="J7">
+        <v>287970</v>
+      </c>
+      <c r="K7">
+        <v>287970</v>
+      </c>
+      <c r="L7">
+        <v>287970</v>
+      </c>
+      <c r="M7">
+        <v>287970</v>
+      </c>
+      <c r="N7">
+        <v>287970</v>
+      </c>
+      <c r="O7">
+        <v>287970</v>
+      </c>
+      <c r="P7">
+        <v>287970</v>
+      </c>
+      <c r="Q7">
+        <v>287970</v>
       </c>
       <c r="R7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1221,44 +1200,44 @@
       <c r="E8" t="s">
         <v>94</v>
       </c>
-      <c r="F8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I8" t="s">
-        <v>105</v>
-      </c>
-      <c r="J8" t="s">
-        <v>105</v>
-      </c>
-      <c r="K8" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" t="s">
-        <v>105</v>
-      </c>
-      <c r="N8" t="s">
-        <v>105</v>
-      </c>
-      <c r="O8" t="s">
-        <v>105</v>
-      </c>
-      <c r="P8" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>105</v>
+      <c r="F8">
+        <v>42995</v>
+      </c>
+      <c r="G8">
+        <v>42995</v>
+      </c>
+      <c r="H8">
+        <v>42995</v>
+      </c>
+      <c r="I8">
+        <v>42995</v>
+      </c>
+      <c r="J8">
+        <v>42995</v>
+      </c>
+      <c r="K8">
+        <v>42995</v>
+      </c>
+      <c r="L8">
+        <v>42995</v>
+      </c>
+      <c r="M8">
+        <v>42995</v>
+      </c>
+      <c r="N8">
+        <v>42995</v>
+      </c>
+      <c r="O8">
+        <v>42995</v>
+      </c>
+      <c r="P8">
+        <v>42995</v>
+      </c>
+      <c r="Q8">
+        <v>42995</v>
       </c>
       <c r="R8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1277,44 +1256,44 @@
       <c r="E9" t="s">
         <v>90</v>
       </c>
-      <c r="F9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J9" t="s">
-        <v>106</v>
-      </c>
-      <c r="K9" t="s">
-        <v>106</v>
-      </c>
-      <c r="L9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N9" t="s">
-        <v>106</v>
-      </c>
-      <c r="O9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>106</v>
+      <c r="F9">
+        <v>116895</v>
+      </c>
+      <c r="G9">
+        <v>116895</v>
+      </c>
+      <c r="H9">
+        <v>116895</v>
+      </c>
+      <c r="I9">
+        <v>116895</v>
+      </c>
+      <c r="J9">
+        <v>116895</v>
+      </c>
+      <c r="K9">
+        <v>116895</v>
+      </c>
+      <c r="L9">
+        <v>116895</v>
+      </c>
+      <c r="M9">
+        <v>116895</v>
+      </c>
+      <c r="N9">
+        <v>116895</v>
+      </c>
+      <c r="O9">
+        <v>116895</v>
+      </c>
+      <c r="P9">
+        <v>116895</v>
+      </c>
+      <c r="Q9">
+        <v>116895</v>
       </c>
       <c r="R9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1333,44 +1312,44 @@
       <c r="E10" t="s">
         <v>89</v>
       </c>
-      <c r="F10" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J10" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" t="s">
-        <v>107</v>
-      </c>
-      <c r="L10" t="s">
-        <v>107</v>
-      </c>
-      <c r="M10" t="s">
-        <v>107</v>
-      </c>
-      <c r="N10" t="s">
-        <v>107</v>
-      </c>
-      <c r="O10" t="s">
-        <v>107</v>
-      </c>
-      <c r="P10" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>107</v>
+      <c r="F10">
+        <v>229950</v>
+      </c>
+      <c r="G10">
+        <v>229950</v>
+      </c>
+      <c r="H10">
+        <v>229950</v>
+      </c>
+      <c r="I10">
+        <v>229950</v>
+      </c>
+      <c r="J10">
+        <v>229950</v>
+      </c>
+      <c r="K10">
+        <v>229950</v>
+      </c>
+      <c r="L10">
+        <v>229950</v>
+      </c>
+      <c r="M10">
+        <v>229950</v>
+      </c>
+      <c r="N10">
+        <v>229950</v>
+      </c>
+      <c r="O10">
+        <v>229950</v>
+      </c>
+      <c r="P10">
+        <v>229950</v>
+      </c>
+      <c r="Q10">
+        <v>229950</v>
       </c>
       <c r="R10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1389,44 +1368,44 @@
       <c r="E11" t="s">
         <v>95</v>
       </c>
-      <c r="F11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I11" t="s">
-        <v>108</v>
-      </c>
-      <c r="J11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K11" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11" t="s">
-        <v>108</v>
-      </c>
-      <c r="M11" t="s">
-        <v>108</v>
-      </c>
-      <c r="N11" t="s">
-        <v>108</v>
-      </c>
-      <c r="O11" t="s">
-        <v>108</v>
-      </c>
-      <c r="P11" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>108</v>
+      <c r="F11">
+        <v>269999</v>
+      </c>
+      <c r="G11">
+        <v>269999</v>
+      </c>
+      <c r="H11">
+        <v>269999</v>
+      </c>
+      <c r="I11">
+        <v>269999</v>
+      </c>
+      <c r="J11">
+        <v>269999</v>
+      </c>
+      <c r="K11">
+        <v>269999</v>
+      </c>
+      <c r="L11">
+        <v>269999</v>
+      </c>
+      <c r="M11">
+        <v>269999</v>
+      </c>
+      <c r="N11">
+        <v>269999</v>
+      </c>
+      <c r="O11">
+        <v>269999</v>
+      </c>
+      <c r="P11">
+        <v>269999</v>
+      </c>
+      <c r="Q11">
+        <v>269999</v>
       </c>
       <c r="R11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1445,44 +1424,11 @@
       <c r="E12" t="s">
         <v>90</v>
       </c>
-      <c r="F12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I12" t="s">
-        <v>109</v>
-      </c>
-      <c r="J12" t="s">
-        <v>109</v>
-      </c>
-      <c r="K12" t="s">
-        <v>109</v>
-      </c>
-      <c r="L12" t="s">
-        <v>109</v>
-      </c>
-      <c r="M12" t="s">
-        <v>109</v>
-      </c>
-      <c r="N12" t="s">
-        <v>109</v>
-      </c>
-      <c r="O12" t="s">
-        <v>109</v>
-      </c>
-      <c r="P12" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>133</v>
+      <c r="Q12">
+        <v>132995</v>
       </c>
       <c r="R12" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1501,44 +1447,44 @@
       <c r="E13" t="s">
         <v>96</v>
       </c>
-      <c r="F13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" t="s">
-        <v>110</v>
-      </c>
-      <c r="H13" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K13" t="s">
-        <v>110</v>
-      </c>
-      <c r="L13" t="s">
-        <v>110</v>
-      </c>
-      <c r="M13" t="s">
-        <v>110</v>
-      </c>
-      <c r="N13" t="s">
-        <v>128</v>
-      </c>
-      <c r="O13" t="s">
-        <v>128</v>
-      </c>
-      <c r="P13" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>128</v>
+      <c r="F13">
+        <v>208000</v>
+      </c>
+      <c r="G13">
+        <v>208000</v>
+      </c>
+      <c r="H13">
+        <v>208000</v>
+      </c>
+      <c r="I13">
+        <v>208000</v>
+      </c>
+      <c r="J13">
+        <v>208000</v>
+      </c>
+      <c r="K13">
+        <v>208000</v>
+      </c>
+      <c r="L13">
+        <v>208000</v>
+      </c>
+      <c r="M13">
+        <v>208000</v>
+      </c>
+      <c r="N13">
+        <v>199000</v>
+      </c>
+      <c r="O13">
+        <v>199000</v>
+      </c>
+      <c r="P13">
+        <v>199000</v>
+      </c>
+      <c r="Q13">
+        <v>199000</v>
       </c>
       <c r="R13" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1549,10 +1495,10 @@
         <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1571,44 +1517,11 @@
       <c r="E15" t="s">
         <v>94</v>
       </c>
-      <c r="F15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" t="s">
-        <v>109</v>
-      </c>
-      <c r="L15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M15" t="s">
-        <v>109</v>
-      </c>
-      <c r="N15" t="s">
-        <v>109</v>
-      </c>
-      <c r="O15" t="s">
-        <v>109</v>
-      </c>
-      <c r="P15" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>111</v>
+      <c r="Q15">
+        <v>229995</v>
       </c>
       <c r="R15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1627,44 +1540,44 @@
       <c r="E16" t="s">
         <v>90</v>
       </c>
-      <c r="F16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" t="s">
-        <v>111</v>
-      </c>
-      <c r="J16" t="s">
-        <v>111</v>
-      </c>
-      <c r="K16" t="s">
-        <v>111</v>
-      </c>
-      <c r="L16" t="s">
-        <v>111</v>
-      </c>
-      <c r="M16" t="s">
-        <v>111</v>
-      </c>
-      <c r="N16" t="s">
-        <v>111</v>
-      </c>
-      <c r="O16" t="s">
-        <v>111</v>
-      </c>
-      <c r="P16" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>111</v>
+      <c r="F16">
+        <v>229995</v>
+      </c>
+      <c r="G16">
+        <v>229995</v>
+      </c>
+      <c r="H16">
+        <v>229995</v>
+      </c>
+      <c r="I16">
+        <v>229995</v>
+      </c>
+      <c r="J16">
+        <v>229995</v>
+      </c>
+      <c r="K16">
+        <v>229995</v>
+      </c>
+      <c r="L16">
+        <v>229995</v>
+      </c>
+      <c r="M16">
+        <v>229995</v>
+      </c>
+      <c r="N16">
+        <v>229995</v>
+      </c>
+      <c r="O16">
+        <v>229995</v>
+      </c>
+      <c r="P16">
+        <v>229995</v>
+      </c>
+      <c r="Q16">
+        <v>229995</v>
       </c>
       <c r="R16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1677,23 +1590,23 @@
       <c r="E17" t="s">
         <v>94</v>
       </c>
-      <c r="F17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J17" t="s">
-        <v>112</v>
+      <c r="F17">
+        <v>137604</v>
+      </c>
+      <c r="G17">
+        <v>137604</v>
+      </c>
+      <c r="H17">
+        <v>137604</v>
+      </c>
+      <c r="I17">
+        <v>137604</v>
+      </c>
+      <c r="J17">
+        <v>137604</v>
       </c>
       <c r="K17" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1712,44 +1625,44 @@
       <c r="E18" t="s">
         <v>90</v>
       </c>
-      <c r="F18" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" t="s">
-        <v>113</v>
-      </c>
-      <c r="J18" t="s">
-        <v>113</v>
-      </c>
-      <c r="K18" t="s">
-        <v>113</v>
-      </c>
-      <c r="L18" t="s">
-        <v>113</v>
-      </c>
-      <c r="M18" t="s">
-        <v>113</v>
-      </c>
-      <c r="N18" t="s">
-        <v>113</v>
-      </c>
-      <c r="O18" t="s">
-        <v>113</v>
-      </c>
-      <c r="P18" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>113</v>
+      <c r="F18">
+        <v>89900</v>
+      </c>
+      <c r="G18">
+        <v>89900</v>
+      </c>
+      <c r="H18">
+        <v>89900</v>
+      </c>
+      <c r="I18">
+        <v>89900</v>
+      </c>
+      <c r="J18">
+        <v>89900</v>
+      </c>
+      <c r="K18">
+        <v>89900</v>
+      </c>
+      <c r="L18">
+        <v>89900</v>
+      </c>
+      <c r="M18">
+        <v>89900</v>
+      </c>
+      <c r="N18">
+        <v>89900</v>
+      </c>
+      <c r="O18">
+        <v>89900</v>
+      </c>
+      <c r="P18">
+        <v>89900</v>
+      </c>
+      <c r="Q18">
+        <v>89900</v>
       </c>
       <c r="R18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1768,44 +1681,44 @@
       <c r="E19" t="s">
         <v>90</v>
       </c>
-      <c r="F19" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" t="s">
-        <v>114</v>
-      </c>
-      <c r="I19" t="s">
-        <v>114</v>
-      </c>
-      <c r="J19" t="s">
-        <v>114</v>
-      </c>
-      <c r="K19" t="s">
-        <v>114</v>
-      </c>
-      <c r="L19" t="s">
-        <v>114</v>
-      </c>
-      <c r="M19" t="s">
-        <v>114</v>
-      </c>
-      <c r="N19" t="s">
-        <v>114</v>
-      </c>
-      <c r="O19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P19" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>114</v>
+      <c r="F19">
+        <v>83500</v>
+      </c>
+      <c r="G19">
+        <v>83500</v>
+      </c>
+      <c r="H19">
+        <v>83500</v>
+      </c>
+      <c r="I19">
+        <v>83500</v>
+      </c>
+      <c r="J19">
+        <v>83500</v>
+      </c>
+      <c r="K19">
+        <v>83500</v>
+      </c>
+      <c r="L19">
+        <v>83500</v>
+      </c>
+      <c r="M19">
+        <v>83500</v>
+      </c>
+      <c r="N19">
+        <v>83500</v>
+      </c>
+      <c r="O19">
+        <v>83500</v>
+      </c>
+      <c r="P19">
+        <v>83500</v>
+      </c>
+      <c r="Q19">
+        <v>83500</v>
       </c>
       <c r="R19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1818,38 +1731,41 @@
       <c r="E20" t="s">
         <v>90</v>
       </c>
-      <c r="F20" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" t="s">
-        <v>115</v>
-      </c>
-      <c r="J20" t="s">
-        <v>115</v>
-      </c>
-      <c r="K20" t="s">
-        <v>115</v>
-      </c>
-      <c r="L20" t="s">
-        <v>115</v>
-      </c>
-      <c r="M20" t="s">
-        <v>115</v>
-      </c>
-      <c r="N20" t="s">
-        <v>115</v>
-      </c>
-      <c r="O20" t="s">
-        <v>115</v>
-      </c>
-      <c r="P20" t="s">
-        <v>115</v>
+      <c r="F20">
+        <v>65995</v>
+      </c>
+      <c r="G20">
+        <v>65995</v>
+      </c>
+      <c r="H20">
+        <v>65995</v>
+      </c>
+      <c r="I20">
+        <v>65995</v>
+      </c>
+      <c r="J20">
+        <v>65995</v>
+      </c>
+      <c r="K20">
+        <v>65995</v>
+      </c>
+      <c r="L20">
+        <v>65995</v>
+      </c>
+      <c r="M20">
+        <v>65995</v>
+      </c>
+      <c r="N20">
+        <v>65995</v>
+      </c>
+      <c r="O20">
+        <v>65995</v>
+      </c>
+      <c r="P20">
+        <v>65995</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1860,10 +1776,10 @@
         <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1874,10 +1790,10 @@
         <v>64</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1896,41 +1812,41 @@
       <c r="E23" t="s">
         <v>90</v>
       </c>
-      <c r="F23" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23" t="s">
-        <v>116</v>
-      </c>
-      <c r="J23" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" t="s">
-        <v>116</v>
-      </c>
-      <c r="M23" t="s">
-        <v>116</v>
-      </c>
-      <c r="N23" t="s">
-        <v>116</v>
-      </c>
-      <c r="O23" t="s">
-        <v>116</v>
-      </c>
-      <c r="P23" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>116</v>
+      <c r="F23">
+        <v>69950</v>
+      </c>
+      <c r="G23">
+        <v>69950</v>
+      </c>
+      <c r="H23">
+        <v>69950</v>
+      </c>
+      <c r="I23">
+        <v>69950</v>
+      </c>
+      <c r="J23">
+        <v>69950</v>
+      </c>
+      <c r="K23">
+        <v>69950</v>
+      </c>
+      <c r="L23">
+        <v>69950</v>
+      </c>
+      <c r="M23">
+        <v>69950</v>
+      </c>
+      <c r="N23">
+        <v>69950</v>
+      </c>
+      <c r="O23">
+        <v>69950</v>
+      </c>
+      <c r="P23">
+        <v>69950</v>
+      </c>
+      <c r="Q23">
+        <v>69950</v>
       </c>
       <c r="R23" t="s">
         <v>116</v>
@@ -1952,41 +1868,41 @@
       <c r="E24" t="s">
         <v>90</v>
       </c>
-      <c r="F24" t="s">
-        <v>117</v>
-      </c>
-      <c r="G24" t="s">
-        <v>117</v>
-      </c>
-      <c r="H24" t="s">
-        <v>117</v>
-      </c>
-      <c r="I24" t="s">
-        <v>117</v>
-      </c>
-      <c r="J24" t="s">
-        <v>117</v>
-      </c>
-      <c r="K24" t="s">
-        <v>117</v>
-      </c>
-      <c r="L24" t="s">
-        <v>117</v>
-      </c>
-      <c r="M24" t="s">
-        <v>117</v>
-      </c>
-      <c r="N24" t="s">
-        <v>117</v>
-      </c>
-      <c r="O24" t="s">
-        <v>117</v>
-      </c>
-      <c r="P24" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>117</v>
+      <c r="F24">
+        <v>89500</v>
+      </c>
+      <c r="G24">
+        <v>89500</v>
+      </c>
+      <c r="H24">
+        <v>89500</v>
+      </c>
+      <c r="I24">
+        <v>89500</v>
+      </c>
+      <c r="J24">
+        <v>89500</v>
+      </c>
+      <c r="K24">
+        <v>89500</v>
+      </c>
+      <c r="L24">
+        <v>89500</v>
+      </c>
+      <c r="M24">
+        <v>89500</v>
+      </c>
+      <c r="N24">
+        <v>89500</v>
+      </c>
+      <c r="O24">
+        <v>89500</v>
+      </c>
+      <c r="P24">
+        <v>89500</v>
+      </c>
+      <c r="Q24">
+        <v>89500</v>
       </c>
       <c r="R24" t="s">
         <v>117</v>
@@ -2008,41 +1924,41 @@
       <c r="E25" t="s">
         <v>90</v>
       </c>
-      <c r="F25" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" t="s">
-        <v>118</v>
-      </c>
-      <c r="I25" t="s">
-        <v>118</v>
-      </c>
-      <c r="J25" t="s">
-        <v>118</v>
-      </c>
-      <c r="K25" t="s">
-        <v>118</v>
-      </c>
-      <c r="L25" t="s">
-        <v>118</v>
-      </c>
-      <c r="M25" t="s">
-        <v>118</v>
-      </c>
-      <c r="N25" t="s">
-        <v>118</v>
-      </c>
-      <c r="O25" t="s">
-        <v>118</v>
-      </c>
-      <c r="P25" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>118</v>
+      <c r="F25">
+        <v>87500</v>
+      </c>
+      <c r="G25">
+        <v>87500</v>
+      </c>
+      <c r="H25">
+        <v>87500</v>
+      </c>
+      <c r="I25">
+        <v>87500</v>
+      </c>
+      <c r="J25">
+        <v>87500</v>
+      </c>
+      <c r="K25">
+        <v>87500</v>
+      </c>
+      <c r="L25">
+        <v>87500</v>
+      </c>
+      <c r="M25">
+        <v>87500</v>
+      </c>
+      <c r="N25">
+        <v>87500</v>
+      </c>
+      <c r="O25">
+        <v>87500</v>
+      </c>
+      <c r="P25">
+        <v>87500</v>
+      </c>
+      <c r="Q25">
+        <v>87500</v>
       </c>
       <c r="R25" t="s">
         <v>118</v>
@@ -2056,10 +1972,10 @@
         <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -2078,41 +1994,41 @@
       <c r="E27" t="s">
         <v>90</v>
       </c>
-      <c r="F27" t="s">
-        <v>119</v>
-      </c>
-      <c r="G27" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" t="s">
-        <v>119</v>
-      </c>
-      <c r="I27" t="s">
-        <v>119</v>
-      </c>
-      <c r="J27" t="s">
-        <v>119</v>
-      </c>
-      <c r="K27" t="s">
-        <v>119</v>
-      </c>
-      <c r="L27" t="s">
-        <v>119</v>
-      </c>
-      <c r="M27" t="s">
-        <v>119</v>
-      </c>
-      <c r="N27" t="s">
-        <v>119</v>
-      </c>
-      <c r="O27" t="s">
-        <v>119</v>
-      </c>
-      <c r="P27" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>119</v>
+      <c r="F27">
+        <v>136990</v>
+      </c>
+      <c r="G27">
+        <v>136990</v>
+      </c>
+      <c r="H27">
+        <v>136990</v>
+      </c>
+      <c r="I27">
+        <v>136990</v>
+      </c>
+      <c r="J27">
+        <v>136990</v>
+      </c>
+      <c r="K27">
+        <v>136990</v>
+      </c>
+      <c r="L27">
+        <v>136990</v>
+      </c>
+      <c r="M27">
+        <v>136990</v>
+      </c>
+      <c r="N27">
+        <v>136990</v>
+      </c>
+      <c r="O27">
+        <v>136990</v>
+      </c>
+      <c r="P27">
+        <v>136990</v>
+      </c>
+      <c r="Q27">
+        <v>136990</v>
       </c>
       <c r="R27" t="s">
         <v>119</v>
@@ -2128,35 +2044,35 @@
       <c r="E28" t="s">
         <v>90</v>
       </c>
-      <c r="F28" t="s">
-        <v>120</v>
-      </c>
-      <c r="G28" t="s">
-        <v>120</v>
-      </c>
-      <c r="H28" t="s">
-        <v>120</v>
-      </c>
-      <c r="I28" t="s">
-        <v>120</v>
-      </c>
-      <c r="J28" t="s">
-        <v>120</v>
-      </c>
-      <c r="K28" t="s">
-        <v>120</v>
-      </c>
-      <c r="L28" t="s">
-        <v>120</v>
-      </c>
-      <c r="M28" t="s">
-        <v>120</v>
-      </c>
-      <c r="N28" t="s">
-        <v>120</v>
+      <c r="F28">
+        <v>147999</v>
+      </c>
+      <c r="G28">
+        <v>147999</v>
+      </c>
+      <c r="H28">
+        <v>147999</v>
+      </c>
+      <c r="I28">
+        <v>147999</v>
+      </c>
+      <c r="J28">
+        <v>147999</v>
+      </c>
+      <c r="K28">
+        <v>147999</v>
+      </c>
+      <c r="L28">
+        <v>147999</v>
+      </c>
+      <c r="M28">
+        <v>147999</v>
+      </c>
+      <c r="N28">
+        <v>147999</v>
       </c>
       <c r="O28" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -2169,17 +2085,17 @@
       <c r="E29" t="s">
         <v>90</v>
       </c>
-      <c r="H29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J29" t="s">
-        <v>126</v>
+      <c r="H29">
+        <v>79660</v>
+      </c>
+      <c r="I29">
+        <v>79660</v>
+      </c>
+      <c r="J29">
+        <v>79660</v>
       </c>
       <c r="K29" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -2198,44 +2114,44 @@
       <c r="E30" t="s">
         <v>96</v>
       </c>
-      <c r="F30" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H30" t="s">
-        <v>121</v>
-      </c>
-      <c r="I30" t="s">
-        <v>121</v>
-      </c>
-      <c r="J30" t="s">
-        <v>121</v>
-      </c>
-      <c r="K30" t="s">
-        <v>121</v>
-      </c>
-      <c r="L30" t="s">
-        <v>121</v>
-      </c>
-      <c r="M30" t="s">
-        <v>121</v>
-      </c>
-      <c r="N30" t="s">
-        <v>121</v>
-      </c>
-      <c r="O30" t="s">
-        <v>121</v>
-      </c>
-      <c r="P30" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>121</v>
+      <c r="F30">
+        <v>124850</v>
+      </c>
+      <c r="G30">
+        <v>124850</v>
+      </c>
+      <c r="H30">
+        <v>124850</v>
+      </c>
+      <c r="I30">
+        <v>124850</v>
+      </c>
+      <c r="J30">
+        <v>124850</v>
+      </c>
+      <c r="K30">
+        <v>124850</v>
+      </c>
+      <c r="L30">
+        <v>124850</v>
+      </c>
+      <c r="M30">
+        <v>124850</v>
+      </c>
+      <c r="N30">
+        <v>124850</v>
+      </c>
+      <c r="O30">
+        <v>124850</v>
+      </c>
+      <c r="P30">
+        <v>124850</v>
+      </c>
+      <c r="Q30">
+        <v>124850</v>
       </c>
       <c r="R30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2254,44 +2170,44 @@
       <c r="E31" t="s">
         <v>90</v>
       </c>
-      <c r="F31" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" t="s">
-        <v>122</v>
-      </c>
-      <c r="H31" t="s">
-        <v>122</v>
-      </c>
-      <c r="I31" t="s">
-        <v>122</v>
-      </c>
-      <c r="J31" t="s">
-        <v>122</v>
-      </c>
-      <c r="K31" t="s">
-        <v>122</v>
-      </c>
-      <c r="L31" t="s">
-        <v>122</v>
-      </c>
-      <c r="M31" t="s">
-        <v>122</v>
-      </c>
-      <c r="N31" t="s">
-        <v>122</v>
-      </c>
-      <c r="O31" t="s">
-        <v>122</v>
-      </c>
-      <c r="P31" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>122</v>
+      <c r="F31">
+        <v>116500</v>
+      </c>
+      <c r="G31">
+        <v>116500</v>
+      </c>
+      <c r="H31">
+        <v>116500</v>
+      </c>
+      <c r="I31">
+        <v>116500</v>
+      </c>
+      <c r="J31">
+        <v>116500</v>
+      </c>
+      <c r="K31">
+        <v>116500</v>
+      </c>
+      <c r="L31">
+        <v>116500</v>
+      </c>
+      <c r="M31">
+        <v>116500</v>
+      </c>
+      <c r="N31">
+        <v>116500</v>
+      </c>
+      <c r="O31">
+        <v>116500</v>
+      </c>
+      <c r="P31">
+        <v>116500</v>
+      </c>
+      <c r="Q31">
+        <v>116500</v>
       </c>
       <c r="R31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2310,44 +2226,44 @@
       <c r="E32" t="s">
         <v>90</v>
       </c>
-      <c r="F32" t="s">
-        <v>123</v>
-      </c>
-      <c r="G32" t="s">
-        <v>123</v>
-      </c>
-      <c r="H32" t="s">
-        <v>123</v>
-      </c>
-      <c r="I32" t="s">
-        <v>123</v>
-      </c>
-      <c r="J32" t="s">
-        <v>123</v>
-      </c>
-      <c r="K32" t="s">
-        <v>123</v>
-      </c>
-      <c r="L32" t="s">
-        <v>123</v>
-      </c>
-      <c r="M32" t="s">
-        <v>123</v>
-      </c>
-      <c r="N32" t="s">
-        <v>123</v>
-      </c>
-      <c r="O32" t="s">
-        <v>123</v>
-      </c>
-      <c r="P32" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>123</v>
+      <c r="F32">
+        <v>144890</v>
+      </c>
+      <c r="G32">
+        <v>144890</v>
+      </c>
+      <c r="H32">
+        <v>144890</v>
+      </c>
+      <c r="I32">
+        <v>144890</v>
+      </c>
+      <c r="J32">
+        <v>144890</v>
+      </c>
+      <c r="K32">
+        <v>144890</v>
+      </c>
+      <c r="L32">
+        <v>144890</v>
+      </c>
+      <c r="M32">
+        <v>144890</v>
+      </c>
+      <c r="N32">
+        <v>144890</v>
+      </c>
+      <c r="O32">
+        <v>144890</v>
+      </c>
+      <c r="P32">
+        <v>144890</v>
+      </c>
+      <c r="Q32">
+        <v>144890</v>
       </c>
       <c r="R32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2366,32 +2282,32 @@
       <c r="E33" t="s">
         <v>90</v>
       </c>
-      <c r="J33" t="s">
-        <v>127</v>
-      </c>
-      <c r="K33" t="s">
-        <v>127</v>
-      </c>
-      <c r="L33" t="s">
-        <v>127</v>
-      </c>
-      <c r="M33" t="s">
-        <v>127</v>
-      </c>
-      <c r="N33" t="s">
-        <v>127</v>
-      </c>
-      <c r="O33" t="s">
-        <v>127</v>
-      </c>
-      <c r="P33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>127</v>
+      <c r="J33">
+        <v>214995</v>
+      </c>
+      <c r="K33">
+        <v>214995</v>
+      </c>
+      <c r="L33">
+        <v>214995</v>
+      </c>
+      <c r="M33">
+        <v>214995</v>
+      </c>
+      <c r="N33">
+        <v>214995</v>
+      </c>
+      <c r="O33">
+        <v>214995</v>
+      </c>
+      <c r="P33">
+        <v>214995</v>
+      </c>
+      <c r="Q33">
+        <v>214995</v>
       </c>
       <c r="R33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -2410,20 +2326,20 @@
       <c r="E34" t="s">
         <v>97</v>
       </c>
-      <c r="N34" t="s">
-        <v>129</v>
-      </c>
-      <c r="O34" t="s">
-        <v>132</v>
-      </c>
-      <c r="P34" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>132</v>
+      <c r="N34">
+        <v>79460</v>
+      </c>
+      <c r="O34">
+        <v>79360</v>
+      </c>
+      <c r="P34">
+        <v>79360</v>
+      </c>
+      <c r="Q34">
+        <v>79360</v>
       </c>
       <c r="R34" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -2442,20 +2358,20 @@
       <c r="E35" t="s">
         <v>90</v>
       </c>
-      <c r="N35" t="s">
-        <v>130</v>
-      </c>
-      <c r="O35" t="s">
-        <v>130</v>
-      </c>
-      <c r="P35" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>130</v>
+      <c r="N35">
+        <v>134995</v>
+      </c>
+      <c r="O35">
+        <v>134995</v>
+      </c>
+      <c r="P35">
+        <v>134995</v>
+      </c>
+      <c r="Q35">
+        <v>134995</v>
       </c>
       <c r="R35" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -2474,20 +2390,20 @@
       <c r="E36" t="s">
         <v>98</v>
       </c>
-      <c r="N36" t="s">
-        <v>131</v>
-      </c>
-      <c r="O36" t="s">
-        <v>131</v>
-      </c>
-      <c r="P36" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>131</v>
+      <c r="N36">
+        <v>134948</v>
+      </c>
+      <c r="O36">
+        <v>134948</v>
+      </c>
+      <c r="P36">
+        <v>134948</v>
+      </c>
+      <c r="Q36">
+        <v>134948</v>
       </c>
       <c r="R36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -2504,7 +2420,7 @@
         <v>26100</v>
       </c>
       <c r="R37" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -2521,7 +2437,7 @@
         <v>47500</v>
       </c>
       <c r="R38" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -2538,7 +2454,7 @@
         <v>14700</v>
       </c>
       <c r="R39" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -2555,7 +2471,7 @@
         <v>10041</v>
       </c>
       <c r="R40" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -2572,7 +2488,7 @@
         <v>537</v>
       </c>
       <c r="R41" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to excel_exporter due to pandas updates
</commit_message>
<xml_diff>
--- a/car_info.xlsx
+++ b/car_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="147">
   <si>
     <t>URL</t>
   </si>
@@ -67,6 +67,27 @@
     <t>08/03/2025</t>
   </si>
   <si>
+    <t>09/03/2025</t>
+  </si>
+  <si>
+    <t>10/03/2025</t>
+  </si>
+  <si>
+    <t>11/03/2025</t>
+  </si>
+  <si>
+    <t>12/03/2025</t>
+  </si>
+  <si>
+    <t>13/03/2025</t>
+  </si>
+  <si>
+    <t>16/03/2025</t>
+  </si>
+  <si>
+    <t>17/03/2025</t>
+  </si>
+  <si>
     <t>https://www.autotrader.co.uk/car-details/202302204461549?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
   <si>
@@ -313,6 +334,9 @@
     <t>Black paint with orange interior highlights</t>
   </si>
   <si>
+    <t>White Interior but leather looking loose</t>
+  </si>
+  <si>
     <t>Price not found</t>
   </si>
   <si>
@@ -352,9 +376,6 @@
     <t>£132,995</t>
   </si>
   <si>
-    <t>£199,000</t>
-  </si>
-  <si>
     <t>£229,995</t>
   </si>
   <si>
@@ -388,28 +409,52 @@
     <t>£214,995</t>
   </si>
   <si>
+    <t>£78,960</t>
+  </si>
+  <si>
+    <t>£134,995</t>
+  </si>
+  <si>
+    <t>£134,948</t>
+  </si>
+  <si>
+    <t>£87,990</t>
+  </si>
+  <si>
+    <t>£124,995</t>
+  </si>
+  <si>
+    <t>£130,995</t>
+  </si>
+  <si>
+    <t>£164,990</t>
+  </si>
+  <si>
+    <t>£224,950</t>
+  </si>
+  <si>
+    <t>£68,950</t>
+  </si>
+  <si>
+    <t>£142,995</t>
+  </si>
+  <si>
+    <t>£102,995</t>
+  </si>
+  <si>
     <t>£79,360</t>
   </si>
   <si>
-    <t>£134,995</t>
-  </si>
-  <si>
-    <t>£134,948</t>
-  </si>
-  <si>
-    <t>£87,990</t>
-  </si>
-  <si>
-    <t>£124,995</t>
-  </si>
-  <si>
-    <t>£130,995</t>
-  </si>
-  <si>
-    <t>£164,990</t>
-  </si>
-  <si>
-    <t>£224,950</t>
+    <t>£66,950</t>
+  </si>
+  <si>
+    <t>£134,990</t>
+  </si>
+  <si>
+    <t>£159,950</t>
+  </si>
+  <si>
+    <t>£219,995</t>
   </si>
 </sst>
 </file>
@@ -786,13 +831,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -847,22 +892,43 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D2">
         <v>36000</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F2">
         <v>143995</v>
@@ -900,25 +966,46 @@
       <c r="Q2">
         <v>143995</v>
       </c>
-      <c r="R2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="R2">
+        <v>143995</v>
+      </c>
+      <c r="S2">
+        <v>143995</v>
+      </c>
+      <c r="T2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U2" t="s">
+        <v>109</v>
+      </c>
+      <c r="V2" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" t="s">
+        <v>140</v>
+      </c>
+      <c r="X2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F3">
         <v>177000</v>
@@ -956,25 +1043,46 @@
       <c r="Q3">
         <v>177000</v>
       </c>
-      <c r="R3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="R3">
+        <v>177000</v>
+      </c>
+      <c r="S3">
+        <v>177000</v>
+      </c>
+      <c r="T3" t="s">
+        <v>110</v>
+      </c>
+      <c r="U3" t="s">
+        <v>110</v>
+      </c>
+      <c r="V3" t="s">
+        <v>110</v>
+      </c>
+      <c r="W3" t="s">
+        <v>110</v>
+      </c>
+      <c r="X3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D4">
         <v>5000</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="F4">
         <v>240000</v>
@@ -1012,25 +1120,46 @@
       <c r="Q4">
         <v>235000</v>
       </c>
-      <c r="R4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="R4">
+        <v>235000</v>
+      </c>
+      <c r="S4">
+        <v>235000</v>
+      </c>
+      <c r="T4" t="s">
+        <v>111</v>
+      </c>
+      <c r="U4" t="s">
+        <v>111</v>
+      </c>
+      <c r="V4" t="s">
+        <v>111</v>
+      </c>
+      <c r="W4" t="s">
+        <v>111</v>
+      </c>
+      <c r="X4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <v>13800</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F5">
         <v>97995</v>
@@ -1068,25 +1197,46 @@
       <c r="Q5">
         <v>97995</v>
       </c>
-      <c r="R5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="R5">
+        <v>97995</v>
+      </c>
+      <c r="S5">
+        <v>97995</v>
+      </c>
+      <c r="T5" t="s">
+        <v>112</v>
+      </c>
+      <c r="U5" t="s">
+        <v>112</v>
+      </c>
+      <c r="V5" t="s">
+        <v>141</v>
+      </c>
+      <c r="W5" t="s">
+        <v>141</v>
+      </c>
+      <c r="X5" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>19603</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F6">
         <v>179995</v>
@@ -1124,25 +1274,46 @@
       <c r="Q6">
         <v>179995</v>
       </c>
-      <c r="R6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6">
+        <v>179995</v>
+      </c>
+      <c r="S6">
+        <v>179995</v>
+      </c>
+      <c r="T6" t="s">
+        <v>113</v>
+      </c>
+      <c r="U6" t="s">
+        <v>113</v>
+      </c>
+      <c r="V6" t="s">
+        <v>113</v>
+      </c>
+      <c r="W6" t="s">
+        <v>113</v>
+      </c>
+      <c r="X6" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>3700</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F7">
         <v>287970</v>
@@ -1180,25 +1351,46 @@
       <c r="Q7">
         <v>287970</v>
       </c>
-      <c r="R7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7">
+        <v>287970</v>
+      </c>
+      <c r="S7">
+        <v>287970</v>
+      </c>
+      <c r="T7" t="s">
+        <v>114</v>
+      </c>
+      <c r="U7" t="s">
+        <v>114</v>
+      </c>
+      <c r="V7" t="s">
+        <v>114</v>
+      </c>
+      <c r="W7" t="s">
+        <v>114</v>
+      </c>
+      <c r="X7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>62000</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F8">
         <v>42995</v>
@@ -1236,25 +1428,46 @@
       <c r="Q8">
         <v>42995</v>
       </c>
-      <c r="R8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="R8">
+        <v>42995</v>
+      </c>
+      <c r="S8">
+        <v>42995</v>
+      </c>
+      <c r="T8" t="s">
+        <v>115</v>
+      </c>
+      <c r="U8" t="s">
+        <v>115</v>
+      </c>
+      <c r="V8" t="s">
+        <v>115</v>
+      </c>
+      <c r="W8" t="s">
+        <v>115</v>
+      </c>
+      <c r="X8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D9">
         <v>40723</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F9">
         <v>116895</v>
@@ -1292,25 +1505,46 @@
       <c r="Q9">
         <v>116895</v>
       </c>
-      <c r="R9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="R9">
+        <v>116895</v>
+      </c>
+      <c r="S9">
+        <v>116895</v>
+      </c>
+      <c r="T9" t="s">
+        <v>116</v>
+      </c>
+      <c r="U9" t="s">
+        <v>116</v>
+      </c>
+      <c r="V9" t="s">
+        <v>116</v>
+      </c>
+      <c r="W9" t="s">
+        <v>116</v>
+      </c>
+      <c r="X9" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D10">
         <v>21750</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F10">
         <v>229950</v>
@@ -1348,25 +1582,46 @@
       <c r="Q10">
         <v>229950</v>
       </c>
-      <c r="R10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="R10">
+        <v>229950</v>
+      </c>
+      <c r="S10">
+        <v>229950</v>
+      </c>
+      <c r="T10" t="s">
+        <v>117</v>
+      </c>
+      <c r="U10" t="s">
+        <v>117</v>
+      </c>
+      <c r="V10" t="s">
+        <v>117</v>
+      </c>
+      <c r="W10" t="s">
+        <v>117</v>
+      </c>
+      <c r="X10" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D11">
         <v>24277</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="F11">
         <v>269999</v>
@@ -1404,48 +1659,90 @@
       <c r="Q11">
         <v>269999</v>
       </c>
-      <c r="R11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="R11">
+        <v>269999</v>
+      </c>
+      <c r="S11">
+        <v>269999</v>
+      </c>
+      <c r="T11" t="s">
+        <v>118</v>
+      </c>
+      <c r="U11" t="s">
+        <v>118</v>
+      </c>
+      <c r="V11" t="s">
+        <v>118</v>
+      </c>
+      <c r="W11" t="s">
+        <v>118</v>
+      </c>
+      <c r="X11" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D12">
         <v>20200</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="Q12">
         <v>132995</v>
       </c>
-      <c r="R12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="R12">
+        <v>132995</v>
+      </c>
+      <c r="S12">
+        <v>132995</v>
+      </c>
+      <c r="T12" t="s">
+        <v>119</v>
+      </c>
+      <c r="U12" t="s">
+        <v>119</v>
+      </c>
+      <c r="V12" t="s">
+        <v>119</v>
+      </c>
+      <c r="W12" t="s">
+        <v>119</v>
+      </c>
+      <c r="X12" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D13">
         <v>5100</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F13">
         <v>208000</v>
@@ -1483,62 +1780,89 @@
       <c r="Q13">
         <v>199000</v>
       </c>
-      <c r="R13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="R13">
+        <v>199000</v>
+      </c>
+      <c r="S13">
+        <v>199000</v>
+      </c>
+      <c r="T13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="F14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D15">
         <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="Q15">
         <v>229995</v>
       </c>
-      <c r="R15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="R15">
+        <v>229995</v>
+      </c>
+      <c r="S15">
+        <v>229995</v>
+      </c>
+      <c r="T15" t="s">
+        <v>120</v>
+      </c>
+      <c r="U15" t="s">
+        <v>120</v>
+      </c>
+      <c r="V15" t="s">
+        <v>120</v>
+      </c>
+      <c r="W15" t="s">
+        <v>120</v>
+      </c>
+      <c r="X15" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D16">
         <v>6145</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F16">
         <v>229995</v>
@@ -1576,19 +1900,40 @@
       <c r="Q16">
         <v>229995</v>
       </c>
-      <c r="R16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="R16">
+        <v>229995</v>
+      </c>
+      <c r="S16">
+        <v>229995</v>
+      </c>
+      <c r="T16" t="s">
+        <v>120</v>
+      </c>
+      <c r="U16" t="s">
+        <v>120</v>
+      </c>
+      <c r="V16" t="s">
+        <v>120</v>
+      </c>
+      <c r="W16" t="s">
+        <v>120</v>
+      </c>
+      <c r="X16" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F17">
         <v>137604</v>
@@ -1606,24 +1951,24 @@
         <v>137604</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>18900</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F18">
         <v>89900</v>
@@ -1661,25 +2006,43 @@
       <c r="Q18">
         <v>89900</v>
       </c>
-      <c r="R18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="R18">
+        <v>89900</v>
+      </c>
+      <c r="S18">
+        <v>89900</v>
+      </c>
+      <c r="T18" t="s">
+        <v>121</v>
+      </c>
+      <c r="U18" t="s">
+        <v>121</v>
+      </c>
+      <c r="V18" t="s">
+        <v>121</v>
+      </c>
+      <c r="W18" t="s">
+        <v>121</v>
+      </c>
+      <c r="X18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <v>28000</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F19">
         <v>83500</v>
@@ -1717,19 +2080,40 @@
       <c r="Q19">
         <v>83500</v>
       </c>
-      <c r="R19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="R19">
+        <v>83500</v>
+      </c>
+      <c r="S19">
+        <v>83500</v>
+      </c>
+      <c r="T19" t="s">
+        <v>122</v>
+      </c>
+      <c r="U19" t="s">
+        <v>122</v>
+      </c>
+      <c r="V19" t="s">
+        <v>122</v>
+      </c>
+      <c r="W19" t="s">
+        <v>122</v>
+      </c>
+      <c r="X19" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F20">
         <v>65995</v>
@@ -1765,52 +2149,52 @@
         <v>65995</v>
       </c>
       <c r="Q20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D23">
         <v>24700</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F23">
         <v>69950</v>
@@ -1848,25 +2232,46 @@
       <c r="Q23">
         <v>69950</v>
       </c>
-      <c r="R23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="R23">
+        <v>69950</v>
+      </c>
+      <c r="S23">
+        <v>69950</v>
+      </c>
+      <c r="T23" t="s">
+        <v>123</v>
+      </c>
+      <c r="U23" t="s">
+        <v>139</v>
+      </c>
+      <c r="V23" t="s">
+        <v>139</v>
+      </c>
+      <c r="W23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X23" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D24">
         <v>18095</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F24">
         <v>89500</v>
@@ -1904,25 +2309,46 @@
       <c r="Q24">
         <v>89500</v>
       </c>
-      <c r="R24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="R24">
+        <v>89500</v>
+      </c>
+      <c r="S24">
+        <v>89500</v>
+      </c>
+      <c r="T24" t="s">
+        <v>124</v>
+      </c>
+      <c r="U24" t="s">
+        <v>124</v>
+      </c>
+      <c r="V24" t="s">
+        <v>124</v>
+      </c>
+      <c r="W24" t="s">
+        <v>124</v>
+      </c>
+      <c r="X24" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D25">
         <v>23302</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F25">
         <v>87500</v>
@@ -1960,39 +2386,57 @@
       <c r="Q25">
         <v>87500</v>
       </c>
-      <c r="R25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="R25">
+        <v>87500</v>
+      </c>
+      <c r="S25">
+        <v>87500</v>
+      </c>
+      <c r="T25" t="s">
+        <v>125</v>
+      </c>
+      <c r="U25" t="s">
+        <v>125</v>
+      </c>
+      <c r="V25" t="s">
+        <v>125</v>
+      </c>
+      <c r="W25" t="s">
+        <v>125</v>
+      </c>
+      <c r="X25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="F26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D27">
         <v>26979</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F27">
         <v>136990</v>
@@ -2030,19 +2474,40 @@
       <c r="Q27">
         <v>136990</v>
       </c>
-      <c r="R27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="R27">
+        <v>136990</v>
+      </c>
+      <c r="S27">
+        <v>136990</v>
+      </c>
+      <c r="T27" t="s">
+        <v>126</v>
+      </c>
+      <c r="U27" t="s">
+        <v>126</v>
+      </c>
+      <c r="V27" t="s">
+        <v>126</v>
+      </c>
+      <c r="W27" t="s">
+        <v>126</v>
+      </c>
+      <c r="X27" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F28">
         <v>147999</v>
@@ -2072,18 +2537,18 @@
         <v>147999</v>
       </c>
       <c r="O28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H29">
         <v>79660</v>
@@ -2095,24 +2560,24 @@
         <v>79660</v>
       </c>
       <c r="K29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D30">
         <v>7500</v>
       </c>
       <c r="E30" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F30">
         <v>124850</v>
@@ -2150,25 +2615,46 @@
       <c r="Q30">
         <v>124850</v>
       </c>
-      <c r="R30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="R30">
+        <v>124850</v>
+      </c>
+      <c r="S30">
+        <v>124850</v>
+      </c>
+      <c r="T30" t="s">
+        <v>127</v>
+      </c>
+      <c r="U30" t="s">
+        <v>127</v>
+      </c>
+      <c r="V30" t="s">
+        <v>127</v>
+      </c>
+      <c r="W30" t="s">
+        <v>127</v>
+      </c>
+      <c r="X30" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>23084</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F31">
         <v>116500</v>
@@ -2206,25 +2692,46 @@
       <c r="Q31">
         <v>116500</v>
       </c>
-      <c r="R31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="R31">
+        <v>116500</v>
+      </c>
+      <c r="S31">
+        <v>116500</v>
+      </c>
+      <c r="T31" t="s">
+        <v>128</v>
+      </c>
+      <c r="U31" t="s">
+        <v>128</v>
+      </c>
+      <c r="V31" t="s">
+        <v>128</v>
+      </c>
+      <c r="W31" t="s">
+        <v>128</v>
+      </c>
+      <c r="X31" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D32">
         <v>14500</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F32">
         <v>144890</v>
@@ -2262,25 +2769,46 @@
       <c r="Q32">
         <v>144890</v>
       </c>
-      <c r="R32" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="R32">
+        <v>144890</v>
+      </c>
+      <c r="S32">
+        <v>144890</v>
+      </c>
+      <c r="T32" t="s">
+        <v>129</v>
+      </c>
+      <c r="U32" t="s">
+        <v>129</v>
+      </c>
+      <c r="V32" t="s">
+        <v>129</v>
+      </c>
+      <c r="W32" t="s">
+        <v>129</v>
+      </c>
+      <c r="X32" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D33">
         <v>1600</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="J33">
         <v>214995</v>
@@ -2306,25 +2834,46 @@
       <c r="Q33">
         <v>214995</v>
       </c>
-      <c r="R33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
+      <c r="R33">
+        <v>214995</v>
+      </c>
+      <c r="S33">
+        <v>214995</v>
+      </c>
+      <c r="T33" t="s">
+        <v>130</v>
+      </c>
+      <c r="U33" t="s">
+        <v>130</v>
+      </c>
+      <c r="V33" t="s">
+        <v>130</v>
+      </c>
+      <c r="W33" t="s">
+        <v>130</v>
+      </c>
+      <c r="X33" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D34">
         <v>22000</v>
       </c>
       <c r="E34" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="N34">
         <v>79460</v>
@@ -2338,25 +2887,43 @@
       <c r="Q34">
         <v>79360</v>
       </c>
-      <c r="R34" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
+      <c r="R34">
+        <v>79360</v>
+      </c>
+      <c r="S34">
+        <v>78960</v>
+      </c>
+      <c r="T34" t="s">
+        <v>131</v>
+      </c>
+      <c r="U34" t="s">
+        <v>131</v>
+      </c>
+      <c r="V34" t="s">
+        <v>142</v>
+      </c>
+      <c r="W34" t="s">
+        <v>142</v>
+      </c>
+      <c r="X34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>34300</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N35">
         <v>134995</v>
@@ -2370,25 +2937,46 @@
       <c r="Q35">
         <v>134995</v>
       </c>
-      <c r="R35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="R35">
+        <v>134995</v>
+      </c>
+      <c r="S35">
+        <v>134995</v>
+      </c>
+      <c r="T35" t="s">
+        <v>132</v>
+      </c>
+      <c r="U35" t="s">
+        <v>132</v>
+      </c>
+      <c r="V35" t="s">
+        <v>132</v>
+      </c>
+      <c r="W35" t="s">
+        <v>132</v>
+      </c>
+      <c r="X35" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D36">
         <v>8000</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="N36">
         <v>134948</v>
@@ -2402,93 +2990,234 @@
       <c r="Q36">
         <v>134948</v>
       </c>
-      <c r="R36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18">
+      <c r="R36">
+        <v>134948</v>
+      </c>
+      <c r="S36">
+        <v>134948</v>
+      </c>
+      <c r="T36" t="s">
+        <v>133</v>
+      </c>
+      <c r="U36" t="s">
+        <v>133</v>
+      </c>
+      <c r="V36" t="s">
+        <v>133</v>
+      </c>
+      <c r="W36" t="s">
+        <v>133</v>
+      </c>
+      <c r="X36" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D37">
         <v>26100</v>
       </c>
-      <c r="R37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="R37">
+        <v>87990</v>
+      </c>
+      <c r="S37">
+        <v>87990</v>
+      </c>
+      <c r="T37" t="s">
+        <v>134</v>
+      </c>
+      <c r="U37" t="s">
+        <v>134</v>
+      </c>
+      <c r="V37" t="s">
+        <v>134</v>
+      </c>
+      <c r="W37" t="s">
+        <v>134</v>
+      </c>
+      <c r="X37" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D38">
         <v>47500</v>
       </c>
-      <c r="R38" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
+      <c r="E38" t="s">
+        <v>101</v>
+      </c>
+      <c r="R38">
+        <v>124995</v>
+      </c>
+      <c r="S38">
+        <v>124995</v>
+      </c>
+      <c r="T38" t="s">
+        <v>135</v>
+      </c>
+      <c r="U38" t="s">
+        <v>135</v>
+      </c>
+      <c r="V38" t="s">
+        <v>135</v>
+      </c>
+      <c r="W38" t="s">
+        <v>135</v>
+      </c>
+      <c r="X38" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <v>14700</v>
       </c>
-      <c r="R39" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18">
+      <c r="E39" t="s">
+        <v>97</v>
+      </c>
+      <c r="R39">
+        <v>130995</v>
+      </c>
+      <c r="S39">
+        <v>130995</v>
+      </c>
+      <c r="T39" t="s">
+        <v>136</v>
+      </c>
+      <c r="U39" t="s">
+        <v>136</v>
+      </c>
+      <c r="V39" t="s">
+        <v>136</v>
+      </c>
+      <c r="W39" t="s">
+        <v>136</v>
+      </c>
+      <c r="X39" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D40">
         <v>10041</v>
       </c>
-      <c r="R40" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
+      <c r="E40" t="s">
+        <v>97</v>
+      </c>
+      <c r="R40">
+        <v>164990</v>
+      </c>
+      <c r="S40">
+        <v>164990</v>
+      </c>
+      <c r="T40" t="s">
+        <v>137</v>
+      </c>
+      <c r="U40" t="s">
+        <v>137</v>
+      </c>
+      <c r="V40" t="s">
+        <v>137</v>
+      </c>
+      <c r="W40" t="s">
+        <v>137</v>
+      </c>
+      <c r="X40" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D41">
         <v>537</v>
       </c>
-      <c r="R41" t="s">
-        <v>131</v>
+      <c r="E41" t="s">
+        <v>97</v>
+      </c>
+      <c r="R41">
+        <v>224950</v>
+      </c>
+      <c r="S41">
+        <v>224950</v>
+      </c>
+      <c r="T41" t="s">
+        <v>138</v>
+      </c>
+      <c r="U41" t="s">
+        <v>138</v>
+      </c>
+      <c r="V41" t="s">
+        <v>138</v>
+      </c>
+      <c r="W41" t="s">
+        <v>138</v>
+      </c>
+      <c r="X41" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
had to increase wait time due to slow load speeds affecting the 'sold' if function to not work properly
</commit_message>
<xml_diff>
--- a/car_info.xlsx
+++ b/car_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="162">
   <si>
     <t>URL</t>
   </si>
@@ -88,6 +88,30 @@
     <t>17/03/2025</t>
   </si>
   <si>
+    <t>18/03/2025</t>
+  </si>
+  <si>
+    <t>19/03/2025</t>
+  </si>
+  <si>
+    <t>20/03/2025</t>
+  </si>
+  <si>
+    <t>21/03/2025</t>
+  </si>
+  <si>
+    <t>22/03/2025</t>
+  </si>
+  <si>
+    <t>24/03/2025</t>
+  </si>
+  <si>
+    <t>25/03/2025</t>
+  </si>
+  <si>
+    <t>26/03/2025</t>
+  </si>
+  <si>
     <t>https://www.autotrader.co.uk/car-details/202302204461549?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
   <si>
@@ -208,6 +232,33 @@
     <t>https://www.autotrader.co.uk/car-details/202503059777856?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
   <si>
+    <t>https://www.autotrader.co.uk/car-details/202503130120222?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503140140354?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502199274313?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502058785158?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503150168260?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503200354314?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503170247683?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202501178145053?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502259471660?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
     <t>Mercedes-Benz G Class</t>
   </si>
   <si>
@@ -244,6 +295,9 @@
     <t>McLaren 720S</t>
   </si>
   <si>
+    <t>McLaren GT</t>
+  </si>
+  <si>
     <t>2019 (19 reg)</t>
   </si>
   <si>
@@ -304,6 +358,9 @@
     <t>2023 (72 reg)</t>
   </si>
   <si>
+    <t>2025 (25 reg)</t>
+  </si>
+  <si>
     <t>Brabus</t>
   </si>
   <si>
@@ -343,16 +400,13 @@
     <t>SOLD</t>
   </si>
   <si>
-    <t>£143,995</t>
-  </si>
-  <si>
-    <t>£177,000</t>
+    <t>£142,995</t>
   </si>
   <si>
     <t>£235,000</t>
   </si>
   <si>
-    <t>£97,995</t>
+    <t>£102,995</t>
   </si>
   <si>
     <t>£179,995</t>
@@ -361,9 +415,6 @@
     <t>£287,970</t>
   </si>
   <si>
-    <t>£42,995</t>
-  </si>
-  <si>
     <t>£116,895</t>
   </si>
   <si>
@@ -379,82 +430,76 @@
     <t>£229,995</t>
   </si>
   <si>
-    <t>£89,900</t>
-  </si>
-  <si>
     <t>£83,500</t>
   </si>
   <si>
-    <t>£69,950</t>
+    <t>£66,950</t>
   </si>
   <si>
     <t>£89,500</t>
   </si>
   <si>
+    <t>£134,990</t>
+  </si>
+  <si>
+    <t>£124,850</t>
+  </si>
+  <si>
+    <t>£116,500</t>
+  </si>
+  <si>
+    <t>£144,890</t>
+  </si>
+  <si>
+    <t>£219,995</t>
+  </si>
+  <si>
+    <t>£134,995</t>
+  </si>
+  <si>
+    <t>£134,948</t>
+  </si>
+  <si>
+    <t>£84,990</t>
+  </si>
+  <si>
+    <t>£124,995</t>
+  </si>
+  <si>
+    <t>£130,995</t>
+  </si>
+  <si>
+    <t>£159,950</t>
+  </si>
+  <si>
+    <t>£224,950</t>
+  </si>
+  <si>
+    <t>£199,995</t>
+  </si>
+  <si>
+    <t>£158,950</t>
+  </si>
+  <si>
+    <t>£78,960</t>
+  </si>
+  <si>
     <t>£87,500</t>
   </si>
   <si>
-    <t>£136,990</t>
-  </si>
-  <si>
-    <t>£124,850</t>
-  </si>
-  <si>
-    <t>£116,500</t>
-  </si>
-  <si>
-    <t>£144,890</t>
-  </si>
-  <si>
-    <t>£214,995</t>
-  </si>
-  <si>
-    <t>£78,960</t>
-  </si>
-  <si>
-    <t>£134,995</t>
-  </si>
-  <si>
-    <t>£134,948</t>
-  </si>
-  <si>
-    <t>£87,990</t>
-  </si>
-  <si>
-    <t>£124,995</t>
-  </si>
-  <si>
-    <t>£130,995</t>
-  </si>
-  <si>
-    <t>£164,990</t>
-  </si>
-  <si>
-    <t>£224,950</t>
-  </si>
-  <si>
-    <t>£68,950</t>
-  </si>
-  <si>
-    <t>£142,995</t>
-  </si>
-  <si>
-    <t>£102,995</t>
-  </si>
-  <si>
-    <t>£79,360</t>
-  </si>
-  <si>
-    <t>£66,950</t>
-  </si>
-  <si>
-    <t>£134,990</t>
-  </si>
-  <si>
-    <t>£159,950</t>
-  </si>
-  <si>
-    <t>£219,995</t>
+    <t>£85,149</t>
+  </si>
+  <si>
+    <t>£85,989</t>
+  </si>
+  <si>
+    <t>£89,995</t>
+  </si>
+  <si>
+    <t>£78,460</t>
+  </si>
+  <si>
+    <t>£189,995</t>
   </si>
 </sst>
 </file>
@@ -831,13 +876,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y41"/>
+  <dimension ref="A1:AG50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,22 +958,46 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D2">
         <v>36000</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="F2">
         <v>143995</v>
@@ -972,40 +1041,64 @@
       <c r="S2">
         <v>143995</v>
       </c>
-      <c r="T2" t="s">
-        <v>109</v>
-      </c>
-      <c r="U2" t="s">
-        <v>109</v>
-      </c>
-      <c r="V2" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" t="s">
-        <v>140</v>
-      </c>
-      <c r="X2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="T2">
+        <v>143995</v>
+      </c>
+      <c r="U2">
+        <v>143995</v>
+      </c>
+      <c r="V2">
+        <v>142995</v>
+      </c>
+      <c r="W2">
+        <v>142995</v>
+      </c>
+      <c r="X2">
+        <v>142995</v>
+      </c>
+      <c r="Y2">
+        <v>142995</v>
+      </c>
+      <c r="Z2">
+        <v>142995</v>
+      </c>
+      <c r="AA2">
+        <v>142995</v>
+      </c>
+      <c r="AB2">
+        <v>142995</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F3">
         <v>177000</v>
@@ -1049,40 +1142,46 @@
       <c r="S3">
         <v>177000</v>
       </c>
-      <c r="T3" t="s">
-        <v>110</v>
-      </c>
-      <c r="U3" t="s">
-        <v>110</v>
-      </c>
-      <c r="V3" t="s">
-        <v>110</v>
-      </c>
-      <c r="W3" t="s">
-        <v>110</v>
-      </c>
-      <c r="X3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="T3">
+        <v>177000</v>
+      </c>
+      <c r="U3">
+        <v>177000</v>
+      </c>
+      <c r="V3">
+        <v>177000</v>
+      </c>
+      <c r="W3">
+        <v>177000</v>
+      </c>
+      <c r="X3">
+        <v>177000</v>
+      </c>
+      <c r="Y3">
+        <v>177000</v>
+      </c>
+      <c r="Z3">
+        <v>177000</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="D4">
         <v>5000</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="F4">
         <v>240000</v>
@@ -1126,40 +1225,64 @@
       <c r="S4">
         <v>235000</v>
       </c>
-      <c r="T4" t="s">
-        <v>111</v>
-      </c>
-      <c r="U4" t="s">
-        <v>111</v>
-      </c>
-      <c r="V4" t="s">
-        <v>111</v>
-      </c>
-      <c r="W4" t="s">
-        <v>111</v>
-      </c>
-      <c r="X4" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="T4">
+        <v>235000</v>
+      </c>
+      <c r="U4">
+        <v>235000</v>
+      </c>
+      <c r="V4">
+        <v>235000</v>
+      </c>
+      <c r="W4">
+        <v>235000</v>
+      </c>
+      <c r="X4">
+        <v>235000</v>
+      </c>
+      <c r="Y4">
+        <v>235000</v>
+      </c>
+      <c r="Z4">
+        <v>235000</v>
+      </c>
+      <c r="AA4">
+        <v>235000</v>
+      </c>
+      <c r="AB4">
+        <v>235000</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="D5">
         <v>13800</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="F5">
         <v>97995</v>
@@ -1203,40 +1326,64 @@
       <c r="S5">
         <v>97995</v>
       </c>
-      <c r="T5" t="s">
-        <v>112</v>
-      </c>
-      <c r="U5" t="s">
-        <v>112</v>
-      </c>
-      <c r="V5" t="s">
-        <v>141</v>
-      </c>
-      <c r="W5" t="s">
-        <v>141</v>
-      </c>
-      <c r="X5" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="T5">
+        <v>97995</v>
+      </c>
+      <c r="U5">
+        <v>97995</v>
+      </c>
+      <c r="V5">
+        <v>102995</v>
+      </c>
+      <c r="W5">
+        <v>102995</v>
+      </c>
+      <c r="X5">
+        <v>102995</v>
+      </c>
+      <c r="Y5">
+        <v>102995</v>
+      </c>
+      <c r="Z5">
+        <v>102995</v>
+      </c>
+      <c r="AA5">
+        <v>102995</v>
+      </c>
+      <c r="AB5">
+        <v>102995</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="D6">
         <v>19603</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F6">
         <v>179995</v>
@@ -1280,40 +1427,64 @@
       <c r="S6">
         <v>179995</v>
       </c>
-      <c r="T6" t="s">
-        <v>113</v>
-      </c>
-      <c r="U6" t="s">
-        <v>113</v>
-      </c>
-      <c r="V6" t="s">
-        <v>113</v>
-      </c>
-      <c r="W6" t="s">
-        <v>113</v>
-      </c>
-      <c r="X6" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="T6">
+        <v>179995</v>
+      </c>
+      <c r="U6">
+        <v>179995</v>
+      </c>
+      <c r="V6">
+        <v>179995</v>
+      </c>
+      <c r="W6">
+        <v>179995</v>
+      </c>
+      <c r="X6">
+        <v>179995</v>
+      </c>
+      <c r="Y6">
+        <v>179995</v>
+      </c>
+      <c r="Z6">
+        <v>179995</v>
+      </c>
+      <c r="AA6">
+        <v>179995</v>
+      </c>
+      <c r="AB6">
+        <v>179995</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="D7">
         <v>3700</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="F7">
         <v>287970</v>
@@ -1357,40 +1528,64 @@
       <c r="S7">
         <v>287970</v>
       </c>
-      <c r="T7" t="s">
-        <v>114</v>
-      </c>
-      <c r="U7" t="s">
-        <v>114</v>
-      </c>
-      <c r="V7" t="s">
-        <v>114</v>
-      </c>
-      <c r="W7" t="s">
-        <v>114</v>
-      </c>
-      <c r="X7" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="T7">
+        <v>287970</v>
+      </c>
+      <c r="U7">
+        <v>287970</v>
+      </c>
+      <c r="V7">
+        <v>287970</v>
+      </c>
+      <c r="W7">
+        <v>287970</v>
+      </c>
+      <c r="X7">
+        <v>287970</v>
+      </c>
+      <c r="Y7">
+        <v>287970</v>
+      </c>
+      <c r="Z7">
+        <v>287970</v>
+      </c>
+      <c r="AA7">
+        <v>287970</v>
+      </c>
+      <c r="AB7">
+        <v>287970</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>62000</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="F8">
         <v>42995</v>
@@ -1434,40 +1629,43 @@
       <c r="S8">
         <v>42995</v>
       </c>
-      <c r="T8" t="s">
-        <v>115</v>
-      </c>
-      <c r="U8" t="s">
-        <v>115</v>
-      </c>
-      <c r="V8" t="s">
-        <v>115</v>
-      </c>
-      <c r="W8" t="s">
-        <v>115</v>
-      </c>
-      <c r="X8" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="T8">
+        <v>42995</v>
+      </c>
+      <c r="U8">
+        <v>42995</v>
+      </c>
+      <c r="V8">
+        <v>42995</v>
+      </c>
+      <c r="W8">
+        <v>42995</v>
+      </c>
+      <c r="X8">
+        <v>42995</v>
+      </c>
+      <c r="Y8">
+        <v>42995</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D9">
         <v>40723</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F9">
         <v>116895</v>
@@ -1511,40 +1709,64 @@
       <c r="S9">
         <v>116895</v>
       </c>
-      <c r="T9" t="s">
-        <v>116</v>
-      </c>
-      <c r="U9" t="s">
-        <v>116</v>
-      </c>
-      <c r="V9" t="s">
-        <v>116</v>
-      </c>
-      <c r="W9" t="s">
-        <v>116</v>
-      </c>
-      <c r="X9" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="T9">
+        <v>116895</v>
+      </c>
+      <c r="U9">
+        <v>116895</v>
+      </c>
+      <c r="V9">
+        <v>116895</v>
+      </c>
+      <c r="W9">
+        <v>116895</v>
+      </c>
+      <c r="X9">
+        <v>116895</v>
+      </c>
+      <c r="Y9">
+        <v>116895</v>
+      </c>
+      <c r="Z9">
+        <v>116895</v>
+      </c>
+      <c r="AA9">
+        <v>116895</v>
+      </c>
+      <c r="AB9">
+        <v>116895</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="D10">
         <v>21750</v>
       </c>
       <c r="E10" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="F10">
         <v>229950</v>
@@ -1588,40 +1810,64 @@
       <c r="S10">
         <v>229950</v>
       </c>
-      <c r="T10" t="s">
-        <v>117</v>
-      </c>
-      <c r="U10" t="s">
-        <v>117</v>
-      </c>
-      <c r="V10" t="s">
-        <v>117</v>
-      </c>
-      <c r="W10" t="s">
-        <v>117</v>
-      </c>
-      <c r="X10" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="T10">
+        <v>229950</v>
+      </c>
+      <c r="U10">
+        <v>229950</v>
+      </c>
+      <c r="V10">
+        <v>229950</v>
+      </c>
+      <c r="W10">
+        <v>229950</v>
+      </c>
+      <c r="X10">
+        <v>229950</v>
+      </c>
+      <c r="Y10">
+        <v>229950</v>
+      </c>
+      <c r="Z10">
+        <v>229950</v>
+      </c>
+      <c r="AA10">
+        <v>229950</v>
+      </c>
+      <c r="AB10">
+        <v>229950</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="D11">
         <v>24277</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F11">
         <v>269999</v>
@@ -1665,40 +1911,64 @@
       <c r="S11">
         <v>269999</v>
       </c>
-      <c r="T11" t="s">
-        <v>118</v>
-      </c>
-      <c r="U11" t="s">
-        <v>118</v>
-      </c>
-      <c r="V11" t="s">
-        <v>118</v>
-      </c>
-      <c r="W11" t="s">
-        <v>118</v>
-      </c>
-      <c r="X11" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="T11">
+        <v>269999</v>
+      </c>
+      <c r="U11">
+        <v>269999</v>
+      </c>
+      <c r="V11">
+        <v>269999</v>
+      </c>
+      <c r="W11">
+        <v>269999</v>
+      </c>
+      <c r="X11">
+        <v>269999</v>
+      </c>
+      <c r="Y11">
+        <v>269999</v>
+      </c>
+      <c r="Z11">
+        <v>269999</v>
+      </c>
+      <c r="AA11">
+        <v>269999</v>
+      </c>
+      <c r="AB11">
+        <v>269999</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="D12">
         <v>20200</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="Q12">
         <v>132995</v>
@@ -1709,40 +1979,64 @@
       <c r="S12">
         <v>132995</v>
       </c>
-      <c r="T12" t="s">
-        <v>119</v>
-      </c>
-      <c r="U12" t="s">
-        <v>119</v>
-      </c>
-      <c r="V12" t="s">
-        <v>119</v>
-      </c>
-      <c r="W12" t="s">
-        <v>119</v>
-      </c>
-      <c r="X12" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="T12">
+        <v>132995</v>
+      </c>
+      <c r="U12">
+        <v>132995</v>
+      </c>
+      <c r="V12">
+        <v>132995</v>
+      </c>
+      <c r="W12">
+        <v>132995</v>
+      </c>
+      <c r="X12">
+        <v>132995</v>
+      </c>
+      <c r="Y12">
+        <v>132995</v>
+      </c>
+      <c r="Z12">
+        <v>132995</v>
+      </c>
+      <c r="AA12">
+        <v>132995</v>
+      </c>
+      <c r="AB12">
+        <v>132995</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D13">
         <v>5100</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="F13">
         <v>208000</v>
@@ -1787,38 +2081,38 @@
         <v>199000</v>
       </c>
       <c r="T13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="G14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="Q15">
         <v>229995</v>
@@ -1829,40 +2123,49 @@
       <c r="S15">
         <v>229995</v>
       </c>
-      <c r="T15" t="s">
-        <v>120</v>
-      </c>
-      <c r="U15" t="s">
-        <v>120</v>
-      </c>
-      <c r="V15" t="s">
-        <v>120</v>
-      </c>
-      <c r="W15" t="s">
-        <v>120</v>
-      </c>
-      <c r="X15" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="T15">
+        <v>229995</v>
+      </c>
+      <c r="U15">
+        <v>229995</v>
+      </c>
+      <c r="V15">
+        <v>229995</v>
+      </c>
+      <c r="W15">
+        <v>229995</v>
+      </c>
+      <c r="X15">
+        <v>229995</v>
+      </c>
+      <c r="Y15">
+        <v>229995</v>
+      </c>
+      <c r="Z15">
+        <v>229995</v>
+      </c>
+      <c r="AA15">
+        <v>229995</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D16">
         <v>6145</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F16">
         <v>229995</v>
@@ -1906,34 +2209,58 @@
       <c r="S16">
         <v>229995</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16">
+        <v>229995</v>
+      </c>
+      <c r="U16">
+        <v>229995</v>
+      </c>
+      <c r="V16">
+        <v>229995</v>
+      </c>
+      <c r="W16">
+        <v>229995</v>
+      </c>
+      <c r="X16">
+        <v>229995</v>
+      </c>
+      <c r="Y16">
+        <v>229995</v>
+      </c>
+      <c r="Z16">
+        <v>229995</v>
+      </c>
+      <c r="AA16">
+        <v>229995</v>
+      </c>
+      <c r="AB16">
+        <v>229995</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
         <v>120</v>
-      </c>
-      <c r="U16" t="s">
-        <v>120</v>
-      </c>
-      <c r="V16" t="s">
-        <v>120</v>
-      </c>
-      <c r="W16" t="s">
-        <v>120</v>
-      </c>
-      <c r="X16" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
-      <c r="A17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" t="s">
-        <v>101</v>
       </c>
       <c r="F17">
         <v>137604</v>
@@ -1951,24 +2278,24 @@
         <v>137604</v>
       </c>
       <c r="K17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D18">
         <v>18900</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F18">
         <v>89900</v>
@@ -2012,37 +2339,37 @@
       <c r="S18">
         <v>89900</v>
       </c>
-      <c r="T18" t="s">
-        <v>121</v>
-      </c>
-      <c r="U18" t="s">
-        <v>121</v>
-      </c>
-      <c r="V18" t="s">
-        <v>121</v>
-      </c>
-      <c r="W18" t="s">
-        <v>121</v>
+      <c r="T18">
+        <v>89900</v>
+      </c>
+      <c r="U18">
+        <v>89900</v>
+      </c>
+      <c r="V18">
+        <v>89900</v>
+      </c>
+      <c r="W18">
+        <v>89900</v>
       </c>
       <c r="X18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25">
-      <c r="A19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>90</v>
       </c>
       <c r="D19">
         <v>28000</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F19">
         <v>83500</v>
@@ -2086,34 +2413,58 @@
       <c r="S19">
         <v>83500</v>
       </c>
-      <c r="T19" t="s">
-        <v>122</v>
-      </c>
-      <c r="U19" t="s">
-        <v>122</v>
-      </c>
-      <c r="V19" t="s">
-        <v>122</v>
-      </c>
-      <c r="W19" t="s">
-        <v>122</v>
-      </c>
-      <c r="X19" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="T19">
+        <v>83500</v>
+      </c>
+      <c r="U19">
+        <v>83500</v>
+      </c>
+      <c r="V19">
+        <v>83500</v>
+      </c>
+      <c r="W19">
+        <v>83500</v>
+      </c>
+      <c r="X19">
+        <v>83500</v>
+      </c>
+      <c r="Y19">
+        <v>83500</v>
+      </c>
+      <c r="Z19">
+        <v>83500</v>
+      </c>
+      <c r="AA19">
+        <v>83500</v>
+      </c>
+      <c r="AB19">
+        <v>83500</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
       <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F20">
         <v>65995</v>
@@ -2149,52 +2500,52 @@
         <v>65995</v>
       </c>
       <c r="Q20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D23">
         <v>24700</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F23">
         <v>69950</v>
@@ -2238,40 +2589,61 @@
       <c r="S23">
         <v>69950</v>
       </c>
-      <c r="T23" t="s">
-        <v>123</v>
-      </c>
-      <c r="U23" t="s">
+      <c r="T23">
+        <v>69950</v>
+      </c>
+      <c r="U23">
+        <v>68950</v>
+      </c>
+      <c r="V23">
+        <v>68950</v>
+      </c>
+      <c r="W23">
+        <v>68950</v>
+      </c>
+      <c r="X23">
+        <v>66950</v>
+      </c>
+      <c r="Y23">
+        <v>66950</v>
+      </c>
+      <c r="Z23">
+        <v>66950</v>
+      </c>
+      <c r="AA23">
+        <v>66950</v>
+      </c>
+      <c r="AB23">
+        <v>66950</v>
+      </c>
+      <c r="AC23" t="s">
         <v>139</v>
       </c>
-      <c r="V23" t="s">
+      <c r="AD23" t="s">
         <v>139</v>
       </c>
-      <c r="W23" t="s">
+      <c r="AE23" t="s">
         <v>139</v>
       </c>
-      <c r="X23" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="AF23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D24">
         <v>18095</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F24">
         <v>89500</v>
@@ -2315,40 +2687,64 @@
       <c r="S24">
         <v>89500</v>
       </c>
-      <c r="T24" t="s">
-        <v>124</v>
-      </c>
-      <c r="U24" t="s">
-        <v>124</v>
-      </c>
-      <c r="V24" t="s">
-        <v>124</v>
-      </c>
-      <c r="W24" t="s">
-        <v>124</v>
-      </c>
-      <c r="X24" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="T24">
+        <v>89500</v>
+      </c>
+      <c r="U24">
+        <v>89500</v>
+      </c>
+      <c r="V24">
+        <v>89500</v>
+      </c>
+      <c r="W24">
+        <v>89500</v>
+      </c>
+      <c r="X24">
+        <v>89500</v>
+      </c>
+      <c r="Y24">
+        <v>89500</v>
+      </c>
+      <c r="Z24">
+        <v>89500</v>
+      </c>
+      <c r="AA24">
+        <v>89500</v>
+      </c>
+      <c r="AB24">
+        <v>89500</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D25">
         <v>23302</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F25">
         <v>87500</v>
@@ -2392,51 +2788,51 @@
       <c r="S25">
         <v>87500</v>
       </c>
-      <c r="T25" t="s">
-        <v>125</v>
-      </c>
-      <c r="U25" t="s">
-        <v>125</v>
-      </c>
-      <c r="V25" t="s">
-        <v>125</v>
-      </c>
-      <c r="W25" t="s">
-        <v>125</v>
-      </c>
-      <c r="X25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
+      <c r="T25">
+        <v>87500</v>
+      </c>
+      <c r="U25">
+        <v>87500</v>
+      </c>
+      <c r="V25">
+        <v>87500</v>
+      </c>
+      <c r="W25">
+        <v>87500</v>
+      </c>
+      <c r="X25">
+        <v>87500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="G26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33">
       <c r="A27" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D27">
         <v>26979</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F27">
         <v>136990</v>
@@ -2480,34 +2876,58 @@
       <c r="S27">
         <v>136990</v>
       </c>
-      <c r="T27" t="s">
-        <v>126</v>
-      </c>
-      <c r="U27" t="s">
-        <v>126</v>
-      </c>
-      <c r="V27" t="s">
-        <v>126</v>
-      </c>
-      <c r="W27" t="s">
-        <v>126</v>
-      </c>
-      <c r="X27" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
+      <c r="T27">
+        <v>136990</v>
+      </c>
+      <c r="U27">
+        <v>136990</v>
+      </c>
+      <c r="V27">
+        <v>136990</v>
+      </c>
+      <c r="W27">
+        <v>136990</v>
+      </c>
+      <c r="X27">
+        <v>134990</v>
+      </c>
+      <c r="Y27">
+        <v>134990</v>
+      </c>
+      <c r="Z27">
+        <v>134990</v>
+      </c>
+      <c r="AA27">
+        <v>134990</v>
+      </c>
+      <c r="AB27">
+        <v>134990</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F28">
         <v>147999</v>
@@ -2537,18 +2957,18 @@
         <v>147999</v>
       </c>
       <c r="O28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
       <c r="A29" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="H29">
         <v>79660</v>
@@ -2560,24 +2980,24 @@
         <v>79660</v>
       </c>
       <c r="K29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D30">
         <v>7500</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="F30">
         <v>124850</v>
@@ -2621,40 +3041,64 @@
       <c r="S30">
         <v>124850</v>
       </c>
-      <c r="T30" t="s">
+      <c r="T30">
+        <v>124850</v>
+      </c>
+      <c r="U30">
+        <v>124850</v>
+      </c>
+      <c r="V30">
+        <v>124850</v>
+      </c>
+      <c r="W30">
+        <v>124850</v>
+      </c>
+      <c r="X30">
+        <v>124850</v>
+      </c>
+      <c r="Y30">
+        <v>124850</v>
+      </c>
+      <c r="Z30">
+        <v>124850</v>
+      </c>
+      <c r="AA30">
+        <v>124850</v>
+      </c>
+      <c r="AB30">
+        <v>124850</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG30" t="s">
         <v>127</v>
       </c>
-      <c r="U30" t="s">
-        <v>127</v>
-      </c>
-      <c r="V30" t="s">
-        <v>127</v>
-      </c>
-      <c r="W30" t="s">
-        <v>127</v>
-      </c>
-      <c r="X30" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
+    </row>
+    <row r="31" spans="1:33">
       <c r="A31" s="3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D31">
         <v>23084</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F31">
         <v>116500</v>
@@ -2698,40 +3142,64 @@
       <c r="S31">
         <v>116500</v>
       </c>
-      <c r="T31" t="s">
-        <v>128</v>
-      </c>
-      <c r="U31" t="s">
-        <v>128</v>
-      </c>
-      <c r="V31" t="s">
-        <v>128</v>
-      </c>
-      <c r="W31" t="s">
-        <v>128</v>
-      </c>
-      <c r="X31" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="T31">
+        <v>116500</v>
+      </c>
+      <c r="U31">
+        <v>116500</v>
+      </c>
+      <c r="V31">
+        <v>116500</v>
+      </c>
+      <c r="W31">
+        <v>116500</v>
+      </c>
+      <c r="X31">
+        <v>116500</v>
+      </c>
+      <c r="Y31">
+        <v>116500</v>
+      </c>
+      <c r="Z31">
+        <v>116500</v>
+      </c>
+      <c r="AA31">
+        <v>116500</v>
+      </c>
+      <c r="AB31">
+        <v>116500</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33">
       <c r="A32" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="D32">
         <v>14500</v>
       </c>
       <c r="E32" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="F32">
         <v>144890</v>
@@ -2775,40 +3243,64 @@
       <c r="S32">
         <v>144890</v>
       </c>
-      <c r="T32" t="s">
-        <v>129</v>
-      </c>
-      <c r="U32" t="s">
-        <v>129</v>
-      </c>
-      <c r="V32" t="s">
-        <v>129</v>
-      </c>
-      <c r="W32" t="s">
-        <v>129</v>
-      </c>
-      <c r="X32" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25">
+      <c r="T32">
+        <v>144890</v>
+      </c>
+      <c r="U32">
+        <v>144890</v>
+      </c>
+      <c r="V32">
+        <v>144890</v>
+      </c>
+      <c r="W32">
+        <v>144890</v>
+      </c>
+      <c r="X32">
+        <v>144890</v>
+      </c>
+      <c r="Y32">
+        <v>144890</v>
+      </c>
+      <c r="Z32">
+        <v>144890</v>
+      </c>
+      <c r="AA32">
+        <v>144890</v>
+      </c>
+      <c r="AB32">
+        <v>144890</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D33">
         <v>1600</v>
       </c>
       <c r="E33" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="J33">
         <v>214995</v>
@@ -2840,40 +3332,64 @@
       <c r="S33">
         <v>214995</v>
       </c>
-      <c r="T33" t="s">
-        <v>130</v>
-      </c>
-      <c r="U33" t="s">
-        <v>130</v>
-      </c>
-      <c r="V33" t="s">
-        <v>130</v>
-      </c>
-      <c r="W33" t="s">
-        <v>130</v>
-      </c>
-      <c r="X33" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="T33">
+        <v>214995</v>
+      </c>
+      <c r="U33">
+        <v>214995</v>
+      </c>
+      <c r="V33">
+        <v>214995</v>
+      </c>
+      <c r="W33">
+        <v>214995</v>
+      </c>
+      <c r="X33">
+        <v>214995</v>
+      </c>
+      <c r="Y33">
+        <v>219995</v>
+      </c>
+      <c r="Z33">
+        <v>219995</v>
+      </c>
+      <c r="AA33">
+        <v>219995</v>
+      </c>
+      <c r="AB33">
+        <v>219995</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33">
       <c r="A34" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D34">
         <v>22000</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="N34">
         <v>79460</v>
@@ -2893,37 +3409,37 @@
       <c r="S34">
         <v>78960</v>
       </c>
-      <c r="T34" t="s">
-        <v>131</v>
-      </c>
-      <c r="U34" t="s">
-        <v>131</v>
-      </c>
-      <c r="V34" t="s">
-        <v>142</v>
-      </c>
-      <c r="W34" t="s">
-        <v>142</v>
+      <c r="T34">
+        <v>78960</v>
+      </c>
+      <c r="U34">
+        <v>78960</v>
+      </c>
+      <c r="V34">
+        <v>79360</v>
+      </c>
+      <c r="W34">
+        <v>79360</v>
       </c>
       <c r="X34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33">
       <c r="A35" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="D35">
         <v>34300</v>
       </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="N35">
         <v>134995</v>
@@ -2943,40 +3459,64 @@
       <c r="S35">
         <v>134995</v>
       </c>
-      <c r="T35" t="s">
-        <v>132</v>
-      </c>
-      <c r="U35" t="s">
-        <v>132</v>
-      </c>
-      <c r="V35" t="s">
-        <v>132</v>
-      </c>
-      <c r="W35" t="s">
-        <v>132</v>
-      </c>
-      <c r="X35" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25">
+      <c r="T35">
+        <v>134995</v>
+      </c>
+      <c r="U35">
+        <v>134995</v>
+      </c>
+      <c r="V35">
+        <v>134995</v>
+      </c>
+      <c r="W35">
+        <v>134995</v>
+      </c>
+      <c r="X35">
+        <v>134995</v>
+      </c>
+      <c r="Y35">
+        <v>134995</v>
+      </c>
+      <c r="Z35">
+        <v>134995</v>
+      </c>
+      <c r="AA35">
+        <v>134995</v>
+      </c>
+      <c r="AB35">
+        <v>134995</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33">
       <c r="A36" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="D36">
         <v>8000</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="N36">
         <v>134948</v>
@@ -2996,40 +3536,64 @@
       <c r="S36">
         <v>134948</v>
       </c>
-      <c r="T36" t="s">
-        <v>133</v>
-      </c>
-      <c r="U36" t="s">
-        <v>133</v>
-      </c>
-      <c r="V36" t="s">
-        <v>133</v>
-      </c>
-      <c r="W36" t="s">
-        <v>133</v>
-      </c>
-      <c r="X36" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25">
+      <c r="T36">
+        <v>134948</v>
+      </c>
+      <c r="U36">
+        <v>134948</v>
+      </c>
+      <c r="V36">
+        <v>134948</v>
+      </c>
+      <c r="W36">
+        <v>134948</v>
+      </c>
+      <c r="X36">
+        <v>134948</v>
+      </c>
+      <c r="Y36">
+        <v>134948</v>
+      </c>
+      <c r="Z36">
+        <v>134948</v>
+      </c>
+      <c r="AA36">
+        <v>134948</v>
+      </c>
+      <c r="AB36">
+        <v>134948</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33">
       <c r="A37" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D37">
         <v>26100</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="R37">
         <v>87990</v>
@@ -3037,40 +3601,64 @@
       <c r="S37">
         <v>87990</v>
       </c>
-      <c r="T37" t="s">
-        <v>134</v>
-      </c>
-      <c r="U37" t="s">
-        <v>134</v>
-      </c>
-      <c r="V37" t="s">
-        <v>134</v>
-      </c>
-      <c r="W37" t="s">
-        <v>134</v>
-      </c>
-      <c r="X37" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25">
+      <c r="T37">
+        <v>87990</v>
+      </c>
+      <c r="U37">
+        <v>87990</v>
+      </c>
+      <c r="V37">
+        <v>87990</v>
+      </c>
+      <c r="W37">
+        <v>87990</v>
+      </c>
+      <c r="X37">
+        <v>87990</v>
+      </c>
+      <c r="Y37">
+        <v>87990</v>
+      </c>
+      <c r="Z37">
+        <v>87990</v>
+      </c>
+      <c r="AA37">
+        <v>87990</v>
+      </c>
+      <c r="AB37">
+        <v>84990</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33">
       <c r="A38" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="D38">
         <v>47500</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="R38">
         <v>124995</v>
@@ -3078,40 +3666,64 @@
       <c r="S38">
         <v>124995</v>
       </c>
-      <c r="T38" t="s">
-        <v>135</v>
-      </c>
-      <c r="U38" t="s">
-        <v>135</v>
-      </c>
-      <c r="V38" t="s">
-        <v>135</v>
-      </c>
-      <c r="W38" t="s">
-        <v>135</v>
-      </c>
-      <c r="X38" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25">
+      <c r="T38">
+        <v>124995</v>
+      </c>
+      <c r="U38">
+        <v>124995</v>
+      </c>
+      <c r="V38">
+        <v>124995</v>
+      </c>
+      <c r="W38">
+        <v>124995</v>
+      </c>
+      <c r="X38">
+        <v>124995</v>
+      </c>
+      <c r="Y38">
+        <v>124995</v>
+      </c>
+      <c r="Z38">
+        <v>124995</v>
+      </c>
+      <c r="AA38">
+        <v>124995</v>
+      </c>
+      <c r="AB38">
+        <v>124995</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>149</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33">
       <c r="A39" s="3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="D39">
         <v>14700</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="R39">
         <v>130995</v>
@@ -3119,40 +3731,64 @@
       <c r="S39">
         <v>130995</v>
       </c>
-      <c r="T39" t="s">
-        <v>136</v>
-      </c>
-      <c r="U39" t="s">
-        <v>136</v>
-      </c>
-      <c r="V39" t="s">
-        <v>136</v>
-      </c>
-      <c r="W39" t="s">
-        <v>136</v>
-      </c>
-      <c r="X39" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25">
+      <c r="T39">
+        <v>130995</v>
+      </c>
+      <c r="U39">
+        <v>130995</v>
+      </c>
+      <c r="V39">
+        <v>130995</v>
+      </c>
+      <c r="W39">
+        <v>130995</v>
+      </c>
+      <c r="X39">
+        <v>130995</v>
+      </c>
+      <c r="Y39">
+        <v>130995</v>
+      </c>
+      <c r="Z39">
+        <v>130995</v>
+      </c>
+      <c r="AA39">
+        <v>130995</v>
+      </c>
+      <c r="AB39">
+        <v>130995</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33">
       <c r="A40" s="3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="D40">
         <v>10041</v>
       </c>
       <c r="E40" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="R40">
         <v>164990</v>
@@ -3160,40 +3796,58 @@
       <c r="S40">
         <v>164990</v>
       </c>
-      <c r="T40" t="s">
-        <v>137</v>
-      </c>
-      <c r="U40" t="s">
-        <v>137</v>
-      </c>
-      <c r="V40" t="s">
-        <v>137</v>
-      </c>
-      <c r="W40" t="s">
-        <v>137</v>
-      </c>
-      <c r="X40" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25">
+      <c r="T40">
+        <v>164990</v>
+      </c>
+      <c r="U40">
+        <v>164990</v>
+      </c>
+      <c r="V40">
+        <v>164990</v>
+      </c>
+      <c r="W40">
+        <v>164990</v>
+      </c>
+      <c r="X40">
+        <v>159950</v>
+      </c>
+      <c r="Y40">
+        <v>159950</v>
+      </c>
+      <c r="Z40">
+        <v>159950</v>
+      </c>
+      <c r="AA40">
+        <v>159950</v>
+      </c>
+      <c r="AB40">
+        <v>159950</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33">
       <c r="A41" s="3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D41">
         <v>537</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="R41">
         <v>224950</v>
@@ -3201,23 +3855,305 @@
       <c r="S41">
         <v>224950</v>
       </c>
-      <c r="T41" t="s">
-        <v>138</v>
-      </c>
-      <c r="U41" t="s">
-        <v>138</v>
-      </c>
-      <c r="V41" t="s">
-        <v>138</v>
-      </c>
-      <c r="W41" t="s">
-        <v>138</v>
-      </c>
-      <c r="X41" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>138</v>
+      <c r="T41">
+        <v>224950</v>
+      </c>
+      <c r="U41">
+        <v>224950</v>
+      </c>
+      <c r="V41">
+        <v>224950</v>
+      </c>
+      <c r="W41">
+        <v>224950</v>
+      </c>
+      <c r="X41">
+        <v>224950</v>
+      </c>
+      <c r="Y41">
+        <v>224950</v>
+      </c>
+      <c r="Z41">
+        <v>224950</v>
+      </c>
+      <c r="AA41">
+        <v>224950</v>
+      </c>
+      <c r="AB41">
+        <v>224950</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>152</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33">
+      <c r="A42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42">
+        <v>3500</v>
+      </c>
+      <c r="Z42">
+        <v>209995</v>
+      </c>
+      <c r="AA42">
+        <v>209995</v>
+      </c>
+      <c r="AB42">
+        <v>199995</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33">
+      <c r="A43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43">
+        <v>11000</v>
+      </c>
+      <c r="Z43">
+        <v>156500</v>
+      </c>
+      <c r="AA43">
+        <v>156500</v>
+      </c>
+      <c r="AB43">
+        <v>156500</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33">
+      <c r="A44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44">
+        <v>8265</v>
+      </c>
+      <c r="AA44">
+        <v>158950</v>
+      </c>
+      <c r="AB44">
+        <v>158950</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33">
+      <c r="A45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="AA45">
+        <v>206285</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33">
+      <c r="A46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46">
+        <v>22000</v>
+      </c>
+      <c r="AA46">
+        <v>78960</v>
+      </c>
+      <c r="AB46">
+        <v>78960</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>160</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33">
+      <c r="A47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47">
+        <v>23302</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33">
+      <c r="A48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48">
+        <v>33500</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33">
+      <c r="A49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49">
+        <v>10000</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33">
+      <c r="A50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50">
+        <v>22100</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>159</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3262,6 +4198,15 @@
     <hyperlink ref="A39" r:id="rId38"/>
     <hyperlink ref="A40" r:id="rId39"/>
     <hyperlink ref="A41" r:id="rId40"/>
+    <hyperlink ref="A42" r:id="rId41"/>
+    <hyperlink ref="A43" r:id="rId42"/>
+    <hyperlink ref="A44" r:id="rId43"/>
+    <hyperlink ref="A45" r:id="rId44"/>
+    <hyperlink ref="A46" r:id="rId45"/>
+    <hyperlink ref="A47" r:id="rId46"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="A49" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>